<commit_message>
outputs initially run - need t ochange stackup, but otherwise ok
</commit_message>
<xml_diff>
--- a/Karman Delta Arm/Ancillary Data/Altium Templates/BOM Template.xlsx
+++ b/Karman Delta Arm/Ancillary Data/Altium Templates/BOM Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Altium SANDBOX\Altium Templates\Op Support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\GitHub\AltiumGithub\Karman Delta Arm\Ancillary Data\Altium Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1489509B-07C6-481F-B214-BC399012A4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29336614-D616-437A-A13E-B6744762D3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27690" yWindow="2115" windowWidth="21495" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38310" yWindow="2355" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB BOM" sheetId="1" r:id="rId1"/>
@@ -98,11 +98,6 @@
     <t>Field=a_CopyrightDate</t>
   </si>
   <si>
-    <t>THIS DRAWING REMAINS THE PROPERTY OF OP SUPPORT LTD.
-COPYRIGHT FOR ALL PURPOSES IS VESTED IN OP SUPPORT LTD.
-THE REPRODUCTION OF THIS DRAWING IN WHOLE OR IN PART IS PROHIBITED WITHOUT EXPRESS CONSENT IN WRITING. THIS DESIGN IS OFFERED FOR USE ONLY WITH EQUIPMENT MANUFACTURED OR SPECIFICALLY RECOMMENDED BY OP SUPPORT LTD. RIGHTS ARE RESERVED TO MAKE A CHARGE FOR THE USE OF THIS DESIGN OR ANY PART THEREOF AND SUCH RIGHT SHALL SUBSIST UNLESS AND UNTIL THE SAME SHALL BE EXPRESSLY WAIVED IN WRITING. ACCEPTANCE OF THIS DRAWING WILL BE CONSTRUED AS AN ACCEPTANCE OF THESE CONDITIONS.</t>
-  </si>
-  <si>
     <t>Column=Manufacturer Part Number 1</t>
   </si>
   <si>
@@ -113,6 +108,11 @@
   </si>
   <si>
     <t>Column=Supplier 1</t>
+  </si>
+  <si>
+    <t>THIS DRAWING REMAINS THE PROPERTY OF SUNRIDE.
+COPYRIGHT FOR ALL PURPOSES IS VESTED IN SUNRIDE.
+THE REPRODUCTION OF THIS DRAWING IN WHOLE OR IN PART IS PROHIBITED WITHOUT EXPRESS CONSENT IN WRITING. THIS DESIGN IS OFFERED FOR USE ONLY WITH EQUIPMENT MANUFACTURED OR SPECIFICALLY RECOMMENDED BY SUNRIDE. RIGHTS ARE RESERVED TO MAKE A CHARGE FOR THE USE OF THIS DESIGN OR ANY PART THEREOF AND SUCH RIGHT SHALL SUBSIST UNLESS AND UNTIL THE SAME SHALL BE EXPRESSLY WAIVED IN WRITING. ACCEPTANCE OF THIS DRAWING WILL BE CONSTRUED AS AN ACCEPTANCE OF THESE CONDITIONS.</t>
   </si>
 </sst>
 </file>
@@ -319,15 +319,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>594226</xdr:colOff>
+      <xdr:colOff>899026</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>65793</xdr:rowOff>
+      <xdr:rowOff>145612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>934255</xdr:colOff>
+      <xdr:colOff>1239055</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>45902</xdr:rowOff>
+      <xdr:rowOff>4182</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -355,8 +355,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11824201" y="227718"/>
-          <a:ext cx="1244904" cy="627809"/>
+          <a:off x="12129001" y="307537"/>
+          <a:ext cx="1244904" cy="506270"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -658,8 +658,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD12"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -692,7 +692,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
@@ -788,16 +788,16 @@
         <v>3</v>
       </c>
       <c r="E9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="G9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="H9" s="21" t="s">
         <v>23</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>24</v>
       </c>
       <c r="I9" s="21" t="s">
         <v>1</v>
@@ -2111,8 +2111,8 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.51470588235294112" bottom="0.94488188976377963" header="0" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;F&amp;C&amp;"Arial,Bold"&amp;8Op Support Ltd
-13 Heywood Road, Harrogate HG2 0LU, UK&amp;RPage &amp;P of &amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;F&amp;C&amp;"Arial,Bold"&amp;8Project Sunride
+The Diamond, 32 Leavygreave Rd, Broomhall, Sheffield, UK, S3 7RD&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>